<commit_message>
clase 5 ejemplo deflacion
</commit_message>
<xml_diff>
--- a/Clase 5 - Markdown, loops y funciones/funciones y loops/bases/ipc_trimestral.xlsx
+++ b/Clase 5 - Markdown, loops y funciones/funciones y loops/bases/ipc_trimestral.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\Guido\Trabajo\Repositorios de R\Cursos de R\Curso R_mercado de trabajo\curso_aset\Clase 5 - Markdown, loops y funciones\funciones y loops\bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF405DFE-2EDE-45A3-A648-418F4E956169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62E3D70-1EBE-465D-8486-7919FD5B4E7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,9 +44,6 @@
     <t>Serie</t>
   </si>
   <si>
-    <t>Valor</t>
-  </si>
-  <si>
     <t>2003</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t>anio_trim</t>
+  </si>
+  <si>
+    <t>ipc</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
   <dimension ref="A1:E83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,21 +478,21 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>6.5081732773227996</v>
@@ -504,13 +504,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>6.56421104723466</v>
@@ -522,13 +522,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>6.6240514261022696</v>
@@ -540,13 +540,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <v>6.7549339421415304</v>
@@ -558,13 +558,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>6.8581098958909896</v>
@@ -576,13 +576,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <v>6.94135515579109</v>
@@ -594,13 +594,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <v>7.1652164515215002</v>
@@ -612,13 +612,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <v>7.3484790204753798</v>
@@ -630,13 +630,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>7.5332227072274396</v>
@@ -648,13 +648,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <v>7.7521866547599698</v>
@@ -666,13 +666,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>7.9935927567561604</v>
@@ -684,13 +684,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>8.1852365205549393</v>
@@ -702,13 +702,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14">
         <v>8.3310976452835792</v>
@@ -720,13 +720,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15">
         <v>8.53621958104576</v>
@@ -738,13 +738,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16">
         <v>8.8345557335026701</v>
@@ -756,13 +756,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17">
         <v>9.3023731514134305</v>
@@ -774,13 +774,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18">
         <v>10.0999982111914</v>
@@ -792,13 +792,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>10.706123164917701</v>
@@ -810,13 +810,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>11.2419564118631</v>
@@ -828,13 +828,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21">
         <v>12.2358124207496</v>
@@ -846,13 +846,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22">
         <v>12.816971039843899</v>
@@ -864,13 +864,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23">
         <v>13.186361093320301</v>
@@ -882,13 +882,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24">
         <v>13.5021482886872</v>
@@ -900,13 +900,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25">
         <v>13.9272099921186</v>
@@ -918,13 +918,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26">
         <v>14.317953101725699</v>
@@ -936,13 +936,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27">
         <v>14.951123826181901</v>
@@ -954,13 +954,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28">
         <v>16.0699537241684</v>
@@ -972,13 +972,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D29">
         <v>17.096487585117998</v>
@@ -990,13 +990,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D30">
         <v>17.7764054628135</v>
@@ -1008,13 +1008,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31">
         <v>18.847021973792401</v>
@@ -1026,13 +1026,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D32">
         <v>19.861475416730599</v>
@@ -1044,13 +1044,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D33">
         <v>21.000977810575399</v>
@@ -1062,13 +1062,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D34">
         <v>22.121768098228301</v>
@@ -1080,13 +1080,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D35">
         <v>23.160381793210401</v>
@@ -1098,13 +1098,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D36">
         <v>24.297716738627699</v>
@@ -1116,13 +1116,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D37">
         <v>25.929880138228299</v>
@@ -1134,13 +1134,13 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38">
         <v>27.4802044545755</v>
@@ -1152,13 +1152,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D39">
         <v>28.8134223240633</v>
@@ -1170,13 +1170,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D40">
         <v>30.354103093667899</v>
@@ -1188,13 +1188,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D41">
         <v>32.021415794218797</v>
@@ -1206,13 +1206,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B42" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D42">
         <v>34.384903056803097</v>
@@ -1224,13 +1224,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43">
         <v>36.932903043422002</v>
@@ -1242,13 +1242,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D44">
         <v>41.545758476481303</v>
@@ -1260,13 +1260,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D45">
         <v>45.138291685125097</v>
@@ -1278,13 +1278,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D46">
         <v>47.356712884476302</v>
@@ -1296,13 +1296,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D47">
         <v>49.519890574380703</v>
@@ -1314,13 +1314,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D48">
         <v>52.037183997001598</v>
@@ -1332,13 +1332,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D49">
         <v>55.132579005169497</v>
@@ -1350,13 +1350,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D50">
         <v>58.18170465659</v>
@@ -1368,13 +1368,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D51">
         <v>61.791037671477298</v>
@@ -1386,13 +1386,13 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D52">
         <v>68.955493520927604</v>
@@ -1404,13 +1404,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D53">
         <v>78.689241578890403</v>
@@ -1422,13 +1422,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D54">
         <v>83.462822288693502</v>
@@ -1440,13 +1440,13 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D55">
         <v>87.420523068585297</v>
@@ -1458,13 +1458,13 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D56">
         <v>91.955997632738303</v>
@@ -1476,13 +1476,13 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D57">
         <v>97.839486100162105</v>
@@ -1494,13 +1494,13 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D58">
         <v>102.385177876452</v>
@@ -1512,13 +1512,13 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B59" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D59">
         <v>107.819338390647</v>
@@ -1530,13 +1530,13 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D60">
         <v>115.20497653518601</v>
@@ -1548,13 +1548,13 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D61">
         <v>124.356036225867</v>
@@ -1566,13 +1566,13 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D62">
         <v>138.674913647137</v>
@@ -1584,13 +1584,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D63">
         <v>158.87296844421201</v>
@@ -1602,13 +1602,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D64">
         <v>174.89959917921001</v>
@@ -1620,13 +1620,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D65">
         <v>194.340998341042</v>
@@ -1638,13 +1638,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C66" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D66">
         <v>213.72735726466601</v>
@@ -1656,13 +1656,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B67" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D67">
         <v>241.75364576985601</v>
@@ -1674,13 +1674,13 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D68">
         <v>263.10869716227597</v>
@@ -1692,13 +1692,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D69">
         <v>279.63240266658698</v>
@@ -1710,13 +1710,13 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D70">
         <v>298.78974222993998</v>
@@ -1728,13 +1728,13 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C71" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D71">
         <v>329.698320290928</v>
@@ -1746,13 +1746,13 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D72">
         <v>370.05474421975998</v>
@@ -1764,13 +1764,13 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C73" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D73">
         <v>415.15818199789999</v>
@@ -1782,13 +1782,13 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D74">
         <v>453.84269963510002</v>
@@ -1800,13 +1800,13 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B75" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D75">
         <v>499.15829627135599</v>
@@ -1818,13 +1818,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B76" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C76" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D76">
         <v>565.32064888129696</v>
@@ -1836,13 +1836,13 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C77" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D77">
         <v>668.25306964118204</v>
@@ -1854,13 +1854,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B78" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C78" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D78">
         <v>806.17419187148096</v>
@@ -1872,13 +1872,13 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B79" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D79">
         <v>957.46752304828397</v>
@@ -1890,13 +1890,13 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B80" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D80">
         <v>1141.80389508604</v>
@@ -1908,13 +1908,13 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C81" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D81">
         <v>1423.3701471521699</v>
@@ -1926,13 +1926,13 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C82" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D82">
         <v>1821.0792744048899</v>
@@ -1944,13 +1944,13 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D83">
         <v>2611.90970064267</v>

</xml_diff>